<commit_message>
Char Select, Char Stat Init
</commit_message>
<xml_diff>
--- a/Assets/MyGame/08.DB/StatsDB.xlsx
+++ b/Assets/MyGame/08.DB/StatsDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gimta\Fork\one-to-one\Assets\MyGame\08.DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8382982-F047-4716-9D9A-6F8DC71FF5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF665992-4A47-48AA-8162-8D2F565AC160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="732" windowWidth="20172" windowHeight="11508" xr2:uid="{E0495DAE-A223-44D5-9629-39147D95F472}"/>
   </bookViews>
@@ -62,15 +62,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>armordurability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rogue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dog</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -458,7 +458,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -483,7 +483,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -500,7 +500,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -511,10 +511,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -531,10 +531,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>5</v>

</xml_diff>

<commit_message>
Fix | MapSpawnner && Fix | StatDB
</commit_message>
<xml_diff>
--- a/Assets/MyGame/08.DB/StatsDB.xlsx
+++ b/Assets/MyGame/08.DB/StatsDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gimta\Fork\one-to-one\Assets\MyGame\08.DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5DF12D-5BF2-4BCA-AA83-08D88A35876C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E031DD-C532-48B2-AE93-EE1F2C006F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="732" windowWidth="20172" windowHeight="11508" xr2:uid="{E0495DAE-A223-44D5-9629-39147D95F472}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +71,10 @@
   </si>
   <si>
     <t>dog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curchar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -455,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976AD11-5C37-4DAD-9C5F-251E5ACE676A}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -549,6 +553,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>